<commit_message>
Modified tables of unbiassdness tests
</commit_message>
<xml_diff>
--- a/gdp_revisions_analysis/output/tables/unbiassdness_e_a_tesis.xlsx
+++ b/gdp_revisions_analysis/output/tables/unbiassdness_e_a_tesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb59f80414e38fcc/Documentos/Research Assistant/CIUP/GDP Revisions/GitHub/peru_gdp_revisions/gdp_revisions_analysis/output/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="133" documentId="6_{297CC11D-4E2D-4C9D-862C-32726B7F11A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51F6BB3F-E74F-40F1-89C9-C2424A9005C1}"/>
+  <xr:revisionPtr revIDLastSave="222" documentId="6_{297CC11D-4E2D-4C9D-862C-32726B7F11A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AC9B9F7-25DB-44ED-B081-6B9ACE7104B4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{59A818B8-AC1C-48B4-9EC6-7BF703468C77}"/>
   </bookViews>
@@ -36,17 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="24">
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Media</t>
   </si>
   <si>
-    <t>Horizonte (h)</t>
-  </si>
-  <si>
     <t>PBI</t>
   </si>
   <si>
@@ -98,9 +92,6 @@
     <t>-0.138*</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>P1</t>
   </si>
   <si>
@@ -108,6 +99,21 @@
   </si>
   <si>
     <t>SD</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>0.219*</t>
+  </si>
+  <si>
+    <t>1.123**</t>
+  </si>
+  <si>
+    <t>0.162**</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -188,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -212,10 +218,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -557,49 +560,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{496513D8-45F4-412F-B325-A911B1FC58A0}">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection sqref="A1:F46"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" style="1" customWidth="1"/>
+    <col min="1" max="2" width="3.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="9" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -607,7 +605,7 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>4</v>
       </c>
@@ -618,19 +616,16 @@
         <v>-4.8000000000000001E-2</v>
       </c>
       <c r="D3" s="2">
+        <v>-0.5</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="F3" s="2">
         <v>0.19600000000000001</v>
       </c>
-      <c r="E3" s="2">
-        <v>-0.5</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>7</v>
       </c>
@@ -641,67 +636,58 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D4" s="2">
+        <v>-0.4</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="F4" s="2">
         <v>0.157</v>
       </c>
-      <c r="E4" s="2">
-        <v>-0.4</v>
-      </c>
-      <c r="F4" s="2">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1">
+        <v>26</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2.3E-2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>-0.3</v>
+      </c>
+      <c r="E5" s="2">
         <v>0.4</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+      <c r="F5" s="2">
+        <v>0.13400000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>16</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B6" s="1">
         <v>25</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C6" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D6" s="2">
+        <v>-0.3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="F6" s="2">
         <v>0.13200000000000001</v>
       </c>
-      <c r="E5" s="2">
-        <v>-0.3</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>24</v>
-      </c>
-      <c r="B6" s="1">
-        <v>22</v>
-      </c>
-      <c r="C6" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="D6" s="2">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -709,7 +695,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -717,22 +703,19 @@
         <v>29</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8" s="2">
+        <v>-0.3</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="F8" s="2">
         <v>0.62</v>
       </c>
-      <c r="E8" s="2">
-        <v>-0.3</v>
-      </c>
-      <c r="F8" s="2">
-        <v>2.8</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -740,70 +723,61 @@
         <v>26</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D9" s="2">
+        <v>-0.4</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="F9" s="2">
         <v>0.63100000000000001</v>
       </c>
-      <c r="E9" s="2">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1">
+        <v>26</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="2">
         <v>-0.4</v>
       </c>
-      <c r="F9" s="2">
+      <c r="E10" s="2">
         <v>2.8</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+      <c r="F10" s="2">
+        <v>0.63900000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
         <v>16</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B11" s="1">
         <v>25</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C11" s="2">
         <v>0.192</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D11" s="2">
+        <v>-0.3</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="F11" s="2">
         <v>0.60099999999999998</v>
       </c>
-      <c r="E10" s="2">
-        <v>-0.3</v>
-      </c>
-      <c r="F10" s="2">
-        <v>2.8</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>24</v>
-      </c>
-      <c r="B11" s="1">
-        <v>22</v>
-      </c>
-      <c r="C11" s="2">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0.13300000000000001</v>
-      </c>
-      <c r="E11" s="2">
-        <v>-0.1</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -811,7 +785,7 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -819,22 +793,19 @@
         <v>29</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D13" s="2">
+        <v>-5.9</v>
+      </c>
+      <c r="E13" s="2">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="F13" s="2">
         <v>3.1440000000000001</v>
       </c>
-      <c r="E13" s="2">
-        <v>-5.9</v>
-      </c>
-      <c r="F13" s="2">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>7</v>
       </c>
@@ -845,67 +816,58 @@
         <v>0.91200000000000003</v>
       </c>
       <c r="D14" s="2">
+        <v>-5.8</v>
+      </c>
+      <c r="E14" s="2">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="F14" s="2">
         <v>2.891</v>
       </c>
-      <c r="E14" s="2">
-        <v>-5.8</v>
-      </c>
-      <c r="F14" s="2">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1">
+        <v>26</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="2">
+        <v>-1.5</v>
+      </c>
+      <c r="E15" s="2">
         <v>8.6999999999999993</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
+      <c r="F15" s="2">
+        <v>2.4630000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
         <v>16</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B16" s="1">
         <v>25</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C16" s="2">
         <v>0.35199999999999998</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D16" s="2">
+        <v>-0.6</v>
+      </c>
+      <c r="E16" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="F16" s="2">
         <v>1.127</v>
       </c>
-      <c r="E15" s="2">
-        <v>-0.6</v>
-      </c>
-      <c r="F15" s="2">
-        <v>4.2</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>24</v>
-      </c>
-      <c r="B16" s="1">
-        <v>22</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0.191</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0.89500000000000002</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2">
-        <v>4.2</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -913,7 +875,7 @@
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>4</v>
       </c>
@@ -924,19 +886,16 @@
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="D18" s="2">
+        <v>-0.5</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="F18" s="2">
         <v>0.311</v>
       </c>
-      <c r="E18" s="2">
-        <v>-0.5</v>
-      </c>
-      <c r="F18" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>7</v>
       </c>
@@ -947,67 +906,58 @@
         <v>0.05</v>
       </c>
       <c r="D19" s="2">
+        <v>-0.2</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="F19" s="2">
         <v>0.249</v>
       </c>
-      <c r="E19" s="2">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>12</v>
+      </c>
+      <c r="B20" s="1">
+        <v>26</v>
+      </c>
+      <c r="C20" s="2">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="D20" s="2">
         <v>-0.2</v>
       </c>
-      <c r="F19" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
+      <c r="E20" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.19400000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
         <v>16</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B21" s="1">
         <v>25</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C21" s="2">
         <v>-4.0000000000000001E-3</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D21" s="2">
+        <v>-1.2</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F21" s="2">
         <v>0.316</v>
       </c>
-      <c r="E20" s="2">
-        <v>-1.2</v>
-      </c>
-      <c r="F20" s="2">
-        <v>0.9</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>24</v>
-      </c>
-      <c r="B21" s="1">
-        <v>22</v>
-      </c>
-      <c r="C21" s="2">
-        <v>0</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0</v>
-      </c>
-      <c r="E21" s="2">
-        <v>0</v>
-      </c>
-      <c r="F21" s="2">
-        <v>0</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -1015,7 +965,7 @@
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>4</v>
       </c>
@@ -1023,22 +973,19 @@
         <v>29</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D23" s="2">
+        <v>-0.3</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="F23" s="2">
         <v>0.378</v>
       </c>
-      <c r="E23" s="2">
-        <v>-0.3</v>
-      </c>
-      <c r="F23" s="2">
-        <v>1.4</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>7</v>
       </c>
@@ -1046,70 +993,61 @@
         <v>26</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="2">
+        <v>-0.3</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.36199999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>12</v>
+      </c>
+      <c r="B25" s="1">
+        <v>26</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="2">
+        <v>-0.2</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.34399999999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
         <v>16</v>
       </c>
-      <c r="D24" s="2">
-        <v>0.36199999999999999</v>
-      </c>
-      <c r="E24" s="2">
-        <v>-0.3</v>
-      </c>
-      <c r="F24" s="2">
-        <v>1.4</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>16</v>
-      </c>
-      <c r="B25" s="1">
+      <c r="B26" s="1">
         <v>25</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" s="2">
+      <c r="C26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="2">
+        <v>-0.2</v>
+      </c>
+      <c r="E26" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F26" s="2">
         <v>0.307</v>
       </c>
-      <c r="E25" s="2">
-        <v>-0.2</v>
-      </c>
-      <c r="F25" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
-        <v>24</v>
-      </c>
-      <c r="B26" s="1">
-        <v>22</v>
-      </c>
-      <c r="C26" s="2">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0.122</v>
-      </c>
-      <c r="E26" s="2">
-        <v>0</v>
-      </c>
-      <c r="F26" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -1117,7 +1055,7 @@
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>4</v>
       </c>
@@ -1128,19 +1066,16 @@
         <v>-9.5000000000000001E-2</v>
       </c>
       <c r="D28" s="2">
+        <v>-2.8</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="F28" s="2">
         <v>0.63700000000000001</v>
       </c>
-      <c r="E28" s="2">
-        <v>-2.8</v>
-      </c>
-      <c r="F28" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>7</v>
       </c>
@@ -1151,67 +1086,58 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="D29" s="2">
+        <v>-0.2</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="F29" s="2">
         <v>0.17799999999999999</v>
       </c>
-      <c r="E29" s="2">
-        <v>-0.2</v>
-      </c>
-      <c r="F29" s="2">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>12</v>
+      </c>
+      <c r="B30" s="1">
+        <v>21</v>
+      </c>
+      <c r="C30" s="2">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="D30" s="2">
+        <v>-0.1</v>
+      </c>
+      <c r="E30" s="2">
         <v>0.7</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
+      <c r="F30" s="2">
+        <v>0.16900000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
         <v>16</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B31" s="1">
         <v>19</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C31" s="2">
         <v>1.6E-2</v>
-      </c>
-      <c r="D30" s="2">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="E30" s="2">
-        <v>0</v>
-      </c>
-      <c r="F30" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
-        <v>24</v>
-      </c>
-      <c r="B31" s="1">
-        <v>18</v>
-      </c>
-      <c r="C31" s="2">
-        <v>0</v>
       </c>
       <c r="D31" s="2">
         <v>0</v>
       </c>
       <c r="E31" s="2">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="F31" s="2">
-        <v>0</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+        <v>6.9000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -1219,7 +1145,7 @@
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>4</v>
       </c>
@@ -1230,19 +1156,16 @@
         <v>-2.1000000000000001E-2</v>
       </c>
       <c r="D33" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E33" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="F33" s="2">
         <v>0.432</v>
       </c>
-      <c r="E33" s="2">
-        <v>-1</v>
-      </c>
-      <c r="F33" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>7</v>
       </c>
@@ -1253,67 +1176,58 @@
         <v>6.2E-2</v>
       </c>
       <c r="D34" s="2">
+        <v>-0.7</v>
+      </c>
+      <c r="E34" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="F34" s="2">
         <v>0.38500000000000001</v>
       </c>
-      <c r="E34" s="2">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>12</v>
+      </c>
+      <c r="B35" s="1">
+        <v>26</v>
+      </c>
+      <c r="C35" s="2">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D35" s="2">
         <v>-0.7</v>
       </c>
-      <c r="F34" s="2">
+      <c r="E35" s="2">
         <v>1.5</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
+      <c r="F35" s="2">
+        <v>0.371</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
         <v>16</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B36" s="1">
         <v>25</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C36" s="2">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D36" s="2">
+        <v>-0.3</v>
+      </c>
+      <c r="E36" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="F36" s="2">
         <v>0.31</v>
       </c>
-      <c r="E35" s="2">
-        <v>-0.3</v>
-      </c>
-      <c r="F35" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
-        <v>24</v>
-      </c>
-      <c r="B36" s="1">
-        <v>22</v>
-      </c>
-      <c r="C36" s="2">
-        <v>0</v>
-      </c>
-      <c r="D36" s="2">
-        <v>0</v>
-      </c>
-      <c r="E36" s="2">
-        <v>0</v>
-      </c>
-      <c r="F36" s="2">
-        <v>0</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -1321,7 +1235,7 @@
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>4</v>
       </c>
@@ -1332,19 +1246,16 @@
         <v>-7.1999999999999995E-2</v>
       </c>
       <c r="D38" s="2">
+        <v>-0.9</v>
+      </c>
+      <c r="E38" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F38" s="2">
         <v>0.437</v>
       </c>
-      <c r="E38" s="2">
-        <v>-0.9</v>
-      </c>
-      <c r="F38" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>7</v>
       </c>
@@ -1355,67 +1266,58 @@
         <v>0.104</v>
       </c>
       <c r="D39" s="2">
+        <v>-0.6</v>
+      </c>
+      <c r="E39" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F39" s="2">
         <v>0.42899999999999999</v>
       </c>
-      <c r="E39" s="2">
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>12</v>
+      </c>
+      <c r="B40" s="1">
+        <v>26</v>
+      </c>
+      <c r="C40" s="2">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="D40" s="2">
         <v>-0.6</v>
       </c>
-      <c r="F39" s="2">
+      <c r="E40" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="1">
+      <c r="F40" s="2">
+        <v>0.40400000000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
         <v>16</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B41" s="1">
         <v>25</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C41" s="2">
         <v>0.06</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D41" s="2">
+        <v>-0.5</v>
+      </c>
+      <c r="E41" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F41" s="2">
         <v>0.34899999999999998</v>
       </c>
-      <c r="E40" s="2">
-        <v>-0.5</v>
-      </c>
-      <c r="F40" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="1">
-        <v>24</v>
-      </c>
-      <c r="B41" s="1">
-        <v>22</v>
-      </c>
-      <c r="C41" s="2">
-        <v>0</v>
-      </c>
-      <c r="D41" s="2">
-        <v>0</v>
-      </c>
-      <c r="E41" s="2">
-        <v>0</v>
-      </c>
-      <c r="F41" s="2">
-        <v>0</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -1423,7 +1325,7 @@
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>4</v>
       </c>
@@ -1431,88 +1333,76 @@
         <v>28</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D43" s="4">
+        <v>-1.4</v>
+      </c>
+      <c r="E43" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="F43" s="4">
         <v>0.46</v>
       </c>
-      <c r="E43" s="4">
-        <v>-1.4</v>
-      </c>
-      <c r="F43" s="4">
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="9">
+        <v>7</v>
+      </c>
+      <c r="B44" s="9">
+        <v>26</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="10">
+        <v>-1.3</v>
+      </c>
+      <c r="E44" s="10">
         <v>0.6</v>
       </c>
-      <c r="G43" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="10">
-        <v>7</v>
-      </c>
-      <c r="B44" s="10">
-        <v>26</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D44" s="11">
+      <c r="F44" s="10">
         <v>0.38200000000000001</v>
       </c>
-      <c r="E44" s="11">
-        <v>-1.3</v>
-      </c>
-      <c r="F44" s="11">
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="9">
+        <v>12</v>
+      </c>
+      <c r="B45" s="9">
+        <v>26</v>
+      </c>
+      <c r="C45" s="10">
+        <v>-6.9000000000000006E-2</v>
+      </c>
+      <c r="D45" s="10">
+        <v>-1</v>
+      </c>
+      <c r="E45" s="10">
         <v>0.6</v>
       </c>
-      <c r="G44" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="10">
+      <c r="F45" s="10">
+        <v>0.313</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="5">
         <v>16</v>
       </c>
-      <c r="B45" s="10">
+      <c r="B46" s="5">
         <v>24</v>
       </c>
-      <c r="C45" s="11">
+      <c r="C46" s="6">
         <v>-0.05</v>
       </c>
-      <c r="D45" s="11">
+      <c r="D46" s="6">
+        <v>-1</v>
+      </c>
+      <c r="E46" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F46" s="6">
         <v>0.309</v>
-      </c>
-      <c r="E45" s="11">
-        <v>-1</v>
-      </c>
-      <c r="F45" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="5">
-        <v>24</v>
-      </c>
-      <c r="B46" s="5">
-        <v>22</v>
-      </c>
-      <c r="C46" s="6">
-        <v>2.7E-2</v>
-      </c>
-      <c r="D46" s="6">
-        <v>0.124</v>
-      </c>
-      <c r="E46" s="6">
-        <v>-0.3</v>
-      </c>
-      <c r="F46" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>